<commit_message>
Final updated to model, and division of calcs and plots file
</commit_message>
<xml_diff>
--- a/data_and_models/Carbon footprints from literature.xlsx
+++ b/data_and_models/Carbon footprints from literature.xlsx
@@ -106,9 +106,6 @@
     <t>Martin Gamboa et al., 2015</t>
   </si>
   <si>
-    <t>A1, average from chart</t>
-  </si>
-  <si>
     <t>Base case (S6)</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>Installed capacity (MW)</t>
+  </si>
+  <si>
+    <t>A1</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E1" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="30"/>
       <c r="G1" s="26"/>
@@ -856,13 +856,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="28"/>
     </row>
@@ -877,12 +877,12 @@
         <v>248</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -892,7 +892,7 @@
         <v>591.57142857142856</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <f>398</f>
@@ -901,7 +901,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -911,7 +911,7 @@
         <v>603</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>465</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -929,7 +929,7 @@
         <v>717.5</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>529</v>
@@ -937,7 +937,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -947,7 +947,7 @@
         <v>795.33333333333337</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>677</v>
@@ -964,7 +964,7 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
@@ -1006,7 +1006,7 @@
         <v>103</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11">
         <v>98.9</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
@@ -1029,10 +1029,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>23.7</v>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
       <c r="E1" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="39"/>
     </row>
@@ -1090,21 +1090,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -1113,18 +1113,18 @@
         <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E3">
         <v>7.5</v>
       </c>
       <c r="F3">
-        <v>1.24</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -1133,18 +1133,18 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4">
         <v>7.5</v>
       </c>
       <c r="F4">
-        <v>1.29</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -1153,7 +1153,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>8.5</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -1173,7 +1173,7 @@
         <v>750</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6">
         <v>9.5</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
@@ -1193,7 +1193,7 @@
         <v>36.700000000000003</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -1213,7 +1213,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
@@ -1233,7 +1233,7 @@
         <v>49.8</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -1253,7 +1253,7 @@
         <v>24.73</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="21">
         <f>((4.21*2580)+(3196*7.08))/(2580+3196)</f>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -1275,7 +1275,7 @@
         <v>46.6</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="21">
         <v>7.23</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>10</v>
@@ -1304,14 +1304,14 @@
     </row>
     <row r="13" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="37" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1349,13 +1349,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="41" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="42"/>
     </row>
@@ -1365,7 +1365,7 @@
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
       <c r="E2" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="40"/>
     </row>
@@ -1380,18 +1380,18 @@
         <v>2.25</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="23">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>10</v>
@@ -1400,18 +1400,18 @@
         <v>5.6</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="23">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -1420,13 +1420,13 @@
         <v>5.7</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1461,12 +1461,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" s="44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
@@ -1474,24 +1474,24 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="15" t="s">
         <v>21</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>2002</v>
@@ -1525,10 +1525,10 @@
         <v>572</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="7">
         <f>SUMIF(C5:F5,"&lt;&gt;N/A")/2</f>
@@ -1547,10 +1547,10 @@
         <v>550</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="7">
         <f>SUMIF(C6:F6,"&lt;&gt;N/A")/2</f>
@@ -1569,10 +1569,10 @@
         <v>683</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="7">
         <f>SUMIF(C7:F7,"&lt;&gt;N/A")/2</f>
@@ -1585,16 +1585,16 @@
         <v>2007</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="8">
         <v>528</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="7">
         <f>SUMIF(C8:F8,"&lt;&gt;N/A")/1</f>
@@ -1635,7 +1635,7 @@
         <v>682</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="14">
         <v>850</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="8">
         <f>SUMIF(C4:C10, "&lt;&gt; N/A")/7</f>
@@ -1672,7 +1672,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="45">
         <f>SUMIF(D4:F10,"&lt;&gt;N/A")/12</f>
@@ -1683,12 +1683,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -1725,24 +1725,24 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>

</xml_diff>

<commit_message>
added separate simplified model with ch4
</commit_message>
<xml_diff>
--- a/data_and_models/Carbon footprints from literature.xlsx
+++ b/data_and_models/Carbon footprints from literature.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Conventional" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
   <si>
     <t>Technology</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Martin Gamboa et al., 2015</t>
   </si>
   <si>
-    <t>Base case (S6)</t>
-  </si>
-  <si>
     <t>Rule et al., 2009</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
   </si>
   <si>
     <t>Sullivan et al. 2010</t>
-  </si>
-  <si>
-    <t>Base case</t>
   </si>
   <si>
     <t>Binary from high-enthalpy reservoir with wells depths of ~ 400-700m, in a cogeneration plant</t>
@@ -179,24 +173,6 @@
     <t>g/kWh</t>
   </si>
   <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>Case 8</t>
-  </si>
-  <si>
-    <t>Case 2</t>
-  </si>
-  <si>
-    <t>S2 (Installed power is not reported for other scenarios)</t>
-  </si>
-  <si>
     <t>Cannot be used; inventory is aggregated and only net installed power is reported</t>
   </si>
   <si>
@@ -221,9 +197,6 @@
     <t>Installed capacity (MW)</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>Paulillo et al. 2020 (base)</t>
   </si>
   <si>
@@ -303,16 +276,23 @@
   </si>
   <si>
     <t>Double, medium case</t>
+  </si>
+  <si>
+    <t>Installed power is not reported for other scenarios</t>
+  </si>
+  <si>
+    <t>Operational CH4 emissions (g/kWh)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +345,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -445,7 +432,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -531,6 +518,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -834,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,18 +835,19 @@
     <col min="1" max="1" width="38.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="4" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D1" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="26"/>
-    </row>
-    <row r="2" spans="1:7" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E1" s="28"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="1:8" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -864,18 +855,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -883,32 +877,37 @@
       <c r="C3" s="4">
         <v>248</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="4">
+        <f>14900000000/(328000000000000/(1000000 *3.6))</f>
+        <v>163.53658536585368</v>
+      </c>
+      <c r="E3" s="38">
+        <f>84600000/(328000000000000/(1000000 *3.6))</f>
+        <v>0.92853658536585371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4">
         <f>'Bravi&amp;Basosi'!C11</f>
-        <v>591.57142857142856</v>
+        <v>690.16666666666663</v>
       </c>
       <c r="D4">
         <f>398</f>
         <v>398</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="38">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -920,13 +919,13 @@
       <c r="D5">
         <v>465</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="38">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -938,13 +937,13 @@
       <c r="D6">
         <v>529</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="38">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -956,44 +955,50 @@
       <c r="D7">
         <v>677</v>
       </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="38">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>47</v>
@@ -1001,10 +1006,14 @@
       <c r="D10">
         <v>41.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="37">
+        <f>0.00000326*1000</f>
+        <v>3.2600000000000003E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -1015,13 +1024,16 @@
       <c r="D11">
         <v>98.9</v>
       </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="39">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
@@ -1033,13 +1045,16 @@
         <f>1470/225.5*3.6</f>
         <v>23.467849223946786</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="38">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>23.7</v>
@@ -1048,13 +1063,36 @@
         <f>1470/253.3*3.6</f>
         <v>20.892222660876431</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="38">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="30" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="7"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="30" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="82" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1065,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,12 +1122,12 @@
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
-      <c r="D1" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="D1" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
       <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1100,19 +1138,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>2</v>
@@ -1120,7 +1158,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1140,13 +1178,10 @@
       <c r="G3">
         <v>100</v>
       </c>
-      <c r="H3" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1166,13 +1201,10 @@
       <c r="G4">
         <v>100</v>
       </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1192,13 +1224,10 @@
       <c r="G5">
         <v>100</v>
       </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1218,13 +1247,10 @@
       <c r="G6">
         <v>100</v>
       </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -1244,13 +1270,10 @@
       <c r="G7">
         <v>100</v>
       </c>
-      <c r="H7" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
@@ -1270,13 +1293,10 @@
       <c r="G8">
         <v>100</v>
       </c>
-      <c r="H8" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
@@ -1296,13 +1316,10 @@
       <c r="G9">
         <v>100</v>
       </c>
-      <c r="H9" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
@@ -1324,12 +1341,12 @@
         <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
@@ -1350,13 +1367,10 @@
       <c r="G11">
         <v>100</v>
       </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
@@ -1380,7 +1394,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
@@ -1404,7 +1418,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
@@ -1426,12 +1440,12 @@
         <v>100</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
@@ -1453,7 +1467,7 @@
         <v>100</v>
       </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1464,13 +1478,13 @@
     </row>
     <row r="17" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1501,32 +1515,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="C1" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="40"/>
+      <c r="E1" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="38"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -1539,18 +1553,18 @@
         <v>2.25</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" s="23">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>5</v>
@@ -1559,18 +1573,18 @@
         <v>5.6</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E4" s="23">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -1579,13 +1593,13 @@
         <v>5.7</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1606,7 +1620,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,37 +1634,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
-        <v>9</v>
+      <c r="A4" s="44" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>2002</v>
@@ -1673,7 +1687,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="1">
         <v>2004</v>
       </c>
@@ -1684,10 +1698,10 @@
         <v>572</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="7">
         <f>SUMIF(C5:F5,"&lt;&gt;N/A")/2</f>
@@ -1695,7 +1709,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="1">
         <v>2005</v>
       </c>
@@ -1706,10 +1720,10 @@
         <v>550</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="7">
         <f>SUMIF(C6:F6,"&lt;&gt;N/A")/2</f>
@@ -1717,7 +1731,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="1">
         <v>2006</v>
       </c>
@@ -1728,10 +1742,10 @@
         <v>683</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="7">
         <f>SUMIF(C7:F7,"&lt;&gt;N/A")/2</f>
@@ -1739,21 +1753,21 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="1">
         <v>2007</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="8">
         <v>528</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="7">
         <f>SUMIF(C8:F8,"&lt;&gt;N/A")/1</f>
@@ -1761,7 +1775,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="1">
         <v>2008</v>
       </c>
@@ -1783,7 +1797,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="9">
         <v>2009</v>
       </c>
@@ -1794,7 +1808,7 @@
         <v>682</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="14">
         <v>850</v>
@@ -1806,11 +1820,11 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="8">
-        <f>SUMIF(C4:C10, "&lt;&gt; N/A")/7</f>
-        <v>591.57142857142856</v>
+        <f>SUMIF(C4:C10, "&lt;&gt; N/A")/6</f>
+        <v>690.16666666666663</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" ref="D11" si="0">SUMIF(D4:D10, "&lt;&gt; N/A")/7</f>
@@ -1831,23 +1845,23 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="43">
+        <v>16</v>
+      </c>
+      <c r="D12" s="46">
         <f>SUMIF(D4:F10,"&lt;&gt;N/A")/12</f>
         <v>670.16666666666663</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -1884,24 +1898,24 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1921,7 +1935,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>

</xml_diff>

<commit_message>
updated plots scripts, changed carbon footprint excel, and removed plot_gsa_results in view of merge
</commit_message>
<xml_diff>
--- a/data_and_models/Carbon footprints from literature.xlsx
+++ b/data_and_models/Carbon footprints from literature.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Andrea\OneDrive - University College London\S4CE\GSA\Geothermal\data_and_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andpa\OneDrive - University College London\S4CE\GSA\Geothermal\data_and_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_3F9849332A1C2AAFD1A86541A9C2C57F028CAEB8" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E4E75EEE-6CC0-4159-B046-22508CB10FE2}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conventional" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Bravi&amp;Basosi" sheetId="2" r:id="rId4"/>
     <sheet name="IPCC" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Andrea Paulillo</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -287,10 +288,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -432,7 +434,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -542,6 +544,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -823,31 +826,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="38.54296875" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
     <col min="4" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.26953125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D1" s="28" t="s">
         <v>35</v>
       </c>
       <c r="E1" s="28"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="2" spans="1:8" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -867,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>51</v>
       </c>
@@ -886,7 +889,7 @@
         <v>0.92853658536585371</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -905,7 +908,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -923,7 +926,7 @@
         <v>5.45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>54</v>
       </c>
@@ -941,7 +944,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>55</v>
       </c>
@@ -959,7 +962,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
@@ -976,7 +979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
@@ -993,7 +996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>3.2600000000000003E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -1045,11 +1048,11 @@
         <f>1470/225.5*3.6</f>
         <v>23.467849223946786</v>
       </c>
-      <c r="E12" s="38">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="47">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
@@ -1063,36 +1066,36 @@
         <f>1470/253.3*3.6</f>
         <v>20.892222660876431</v>
       </c>
-      <c r="E13" s="38">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="47">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E16" s="7"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D20" s="7"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="30" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="82" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1100,25 +1103,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="28.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1130,7 +1133,7 @@
       <c r="G1" s="40"/>
       <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:8" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>48</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>49</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
@@ -1368,7 +1371,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>42</v>
       </c>
@@ -1392,7 +1395,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -1416,7 +1419,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
@@ -1443,7 +1446,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>65</v>
       </c>
@@ -1470,13 +1473,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="2"/>
       <c r="C16" s="32"/>
       <c r="D16" s="21"/>
     </row>
-    <row r="17" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34" t="s">
         <v>22</v>
       </c>
@@ -1497,24 +1500,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.7265625" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="32.54296875" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
@@ -1532,7 +1535,7 @@
       </c>
       <c r="F1" s="43"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -1542,7 +1545,7 @@
       </c>
       <c r="F2" s="41"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
@@ -1562,7 +1565,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>7</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1616,28 +1619,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C2" s="45" t="s">
         <v>9</v>
       </c>
@@ -1645,7 +1648,7 @@
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C3" s="17" t="s">
         <v>10</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="44" t="s">
         <v>8</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>641.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="44"/>
       <c r="B5" s="1">
         <v>2004</v>
@@ -1708,7 +1711,7 @@
         <v>476.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="44"/>
       <c r="B6" s="1">
         <v>2005</v>
@@ -1730,7 +1733,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="44"/>
       <c r="B7" s="1">
         <v>2006</v>
@@ -1752,7 +1755,7 @@
         <v>645.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="44"/>
       <c r="B8" s="1">
         <v>2007</v>
@@ -1774,7 +1777,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="44"/>
       <c r="B9" s="1">
         <v>2008</v>
@@ -1796,7 +1799,7 @@
         <v>775.75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="44"/>
       <c r="B10" s="9">
         <v>2009</v>
@@ -1818,7 +1821,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>650.03571428571433</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1854,23 +1857,23 @@
       <c r="E12" s="46"/>
       <c r="F12" s="46"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G19" s="7"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" s="19"/>
     </row>
   </sheetData>
@@ -1884,19 +1887,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>30</v>
       </c>
@@ -1951,7 +1954,7 @@
       <c r="M5" s="20"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F2">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F2">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
small changes to plots, and addedd plot for Goldschmidt conference
</commit_message>
<xml_diff>
--- a/data_and_models/Carbon footprints from literature.xlsx
+++ b/data_and_models/Carbon footprints from literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andpa\OneDrive - University College London\S4CE\GSA\Geothermal\data_and_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_3F9849332A1C2AAFD1A86541A9C2C57F028CAEB8" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E4E75EEE-6CC0-4159-B046-22508CB10FE2}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_3F9849332A1C2AAFD1A86541A9C2C57F028CAEB8" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0185A3E7-4222-4026-B3FE-AB887BB470BE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conventional" sheetId="1" r:id="rId1"/>
@@ -264,9 +264,6 @@
     <t>Success rate (%)</t>
   </si>
   <si>
-    <t>Treyer et al. 2015 (Base)</t>
-  </si>
-  <si>
     <t>Bauer et al. 2017 (D-M)</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>Operational CH4 emissions (g/kWh)</t>
+  </si>
+  <si>
+    <t>Treyer et al. 2015 (base)</t>
   </si>
 </sst>
 </file>
@@ -523,6 +523,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -544,7 +545,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -829,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -864,7 +864,7 @@
         <v>37</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>2</v>
@@ -1048,7 +1048,7 @@
         <f>1470/225.5*3.6</f>
         <v>23.467849223946786</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="40">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
         <f>1470/253.3*3.6</f>
         <v>20.892222660876431</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="40">
         <v>3.1E-2</v>
       </c>
     </row>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,12 +1125,12 @@
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1344,7 +1344,7 @@
         <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1397,7 +1397,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
@@ -1443,12 +1443,12 @@
         <v>100</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
@@ -1470,7 +1470,7 @@
         <v>100</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1518,32 +1518,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="43"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="41" t="s">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="41"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
@@ -1641,12 +1641,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C3" s="17" t="s">
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
@@ -1690,7 +1690,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="44"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="1">
         <v>2004</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="44"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="1">
         <v>2005</v>
       </c>
@@ -1734,7 +1734,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="44"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="1">
         <v>2006</v>
       </c>
@@ -1756,7 +1756,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="44"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="1">
         <v>2007</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="44"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="1">
         <v>2008</v>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="44"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="9">
         <v>2009</v>
       </c>
@@ -1850,12 +1850,12 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="47">
         <f>SUMIF(D4:F10,"&lt;&gt;N/A")/12</f>
         <v>670.16666666666663</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
Fixed error in HSD plot, and improved all plots for simplified models (especially fontsizes)
</commit_message>
<xml_diff>
--- a/data_and_models/Carbon footprints from literature.xlsx
+++ b/data_and_models/Carbon footprints from literature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andpa\OneDrive - University College London\S4CE\GSA\Geothermal\data_and_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucecapa_ucl_ac_uk/Documents/Projects/S4CE/GSA/Geothermal/data_and_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_3F9849332A1C2AAFD1A86541A9C2C57F028CAEB8" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0185A3E7-4222-4026-B3FE-AB887BB470BE}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_3F9849332A1C2AAFD1A86541A9C2C57F028CAEB8" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0185A3E7-4222-4026-B3FE-AB887BB470BE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conventional" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -833,24 +836,24 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.54296875" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
     <col min="4" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="27.26953125" customWidth="1"/>
+    <col min="6" max="6" width="27.21875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D1" s="28" t="s">
         <v>35</v>
       </c>
       <c r="E1" s="28"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="2" spans="1:8" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -870,7 +873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>51</v>
       </c>
@@ -889,7 +892,7 @@
         <v>0.92853658536585371</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -908,7 +911,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -926,7 +929,7 @@
         <v>5.45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>54</v>
       </c>
@@ -944,7 +947,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>55</v>
       </c>
@@ -962,7 +965,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
@@ -979,7 +982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
@@ -996,7 +999,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>3.2600000000000003E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
@@ -1070,32 +1073,32 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E16" s="7"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D20" s="7"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="30" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="4:5" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="82" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1106,22 +1109,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" customWidth="1"/>
-    <col min="8" max="8" width="28.26953125" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="8" max="8" width="28.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1133,7 +1136,7 @@
       <c r="G1" s="41"/>
       <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:8" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
@@ -1205,7 +1208,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>48</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>49</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>42</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>69</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>63</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
@@ -1473,13 +1476,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="2"/>
       <c r="C16" s="32"/>
       <c r="D16" s="21"/>
     </row>
-    <row r="17" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>22</v>
       </c>
@@ -1507,17 +1510,17 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="4" max="4" width="32.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
@@ -1535,7 +1538,7 @@
       </c>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -1545,7 +1548,7 @@
       </c>
       <c r="F2" s="42"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>7</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1626,21 +1629,21 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" s="46" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +1651,7 @@
       <c r="E2" s="46"/>
       <c r="F2" s="46"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" s="17" t="s">
         <v>10</v>
       </c>
@@ -1665,7 +1668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="45" t="s">
         <v>8</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>641.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" s="1">
         <v>2004</v>
@@ -1711,7 +1714,7 @@
         <v>476.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="45"/>
       <c r="B6" s="1">
         <v>2005</v>
@@ -1733,7 +1736,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="45"/>
       <c r="B7" s="1">
         <v>2006</v>
@@ -1755,7 +1758,7 @@
         <v>645.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="45"/>
       <c r="B8" s="1">
         <v>2007</v>
@@ -1777,7 +1780,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="45"/>
       <c r="B9" s="1">
         <v>2008</v>
@@ -1799,7 +1802,7 @@
         <v>775.75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="45"/>
       <c r="B10" s="9">
         <v>2009</v>
@@ -1821,7 +1824,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1846,7 +1849,7 @@
         <v>650.03571428571433</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1857,23 +1860,23 @@
       <c r="E12" s="47"/>
       <c r="F12" s="47"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G19" s="7"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="19"/>
     </row>
   </sheetData>
@@ -1890,16 +1893,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -1916,7 +1919,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>30</v>
       </c>

</xml_diff>